<commit_message>
Load & Show Inserate
</commit_message>
<xml_diff>
--- a/dokumentation/zeitplan.xlsx
+++ b/dokumentation/zeitplan.xlsx
@@ -393,6 +393,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,19 +420,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -429,29 +450,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,7 +770,7 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,106 +783,106 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="24">
+      <c r="C1" s="30"/>
+      <c r="D1" s="22">
         <v>1</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="24">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22">
         <v>2</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="24">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="22">
         <v>3</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="24">
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="22">
         <v>4</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="24">
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="22">
         <v>5</v>
       </c>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="26"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="24" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="24" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="24" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="24" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="26"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="24"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29">
+      <c r="C3" s="30"/>
+      <c r="D3" s="36">
         <v>43040</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32">
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="31">
         <v>43041</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32">
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31">
         <v>43042</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="32">
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="31">
         <v>43047</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="32">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="31">
         <v>43049</v>
       </c>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="34"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -937,8 +937,8 @@
         <v>4</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -954,10 +954,10 @@
       <c r="R5" s="14"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="20">
+      <c r="A6" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
@@ -980,8 +980,8 @@
       <c r="R6" s="9"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1002,10 +1002,10 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="25">
         <v>1.2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
@@ -1028,8 +1028,8 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1050,10 +1050,10 @@
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+      <c r="A10" s="25">
         <v>1.3</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1076,8 +1076,8 @@
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1107,10 +1107,10 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -1122,10 +1122,10 @@
       <c r="R12" s="14"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="25">
         <v>2.1</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C13" t="s">
@@ -1148,8 +1148,8 @@
       <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1170,10 +1170,10 @@
       <c r="R14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="20">
+      <c r="A15" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
@@ -1196,8 +1196,8 @@
       <c r="R15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1218,10 +1218,10 @@
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
+      <c r="A17" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
@@ -1244,8 +1244,8 @@
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1266,10 +1266,10 @@
       <c r="R18" s="5"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
+      <c r="A19" s="25">
         <v>2.4</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
@@ -1292,8 +1292,8 @@
       <c r="R19" s="5"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="38"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1338,10 +1338,10 @@
       <c r="R21" s="14"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
+      <c r="A22" s="25">
         <v>3.1</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C22" t="s">
@@ -1364,8 +1364,8 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1386,10 +1386,10 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+      <c r="A24" s="25">
         <v>3.2</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="19" t="s">
@@ -1412,8 +1412,8 @@
       <c r="R24" s="5"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1447,21 +1447,21 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
       <c r="R26" s="14"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
+      <c r="A27" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
@@ -1484,8 +1484,8 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1495,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="1"/>
+      <c r="J28" s="17"/>
       <c r="K28" s="1"/>
       <c r="L28" s="5"/>
       <c r="M28" s="1"/>
@@ -1506,10 +1506,10 @@
       <c r="R28" s="5"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="25">
         <v>4.2</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C29" t="s">
@@ -1532,8 +1532,8 @@
       <c r="R29" s="5"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="1"/>
+      <c r="J30" s="17"/>
       <c r="K30" s="1"/>
       <c r="L30" s="5"/>
       <c r="M30" s="1"/>
@@ -1554,10 +1554,10 @@
       <c r="R30" s="5"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="20">
+      <c r="A31" s="25">
         <v>4.3</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C31" t="s">
@@ -1580,8 +1580,8 @@
       <c r="R31" s="5"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1592,9 +1592,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="5"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="1"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="17"/>
       <c r="N32" s="1"/>
       <c r="O32" s="5"/>
       <c r="P32" s="1"/>
@@ -1602,10 +1602,10 @@
       <c r="R32" s="5"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="20">
+      <c r="A33" s="25">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C33" t="s">
@@ -1628,8 +1628,8 @@
       <c r="R33" s="5"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1642,18 +1642,18 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
       <c r="O34" s="5"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="5"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="20">
+      <c r="A35" s="25">
         <v>4.5</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C35" t="s">
@@ -1676,8 +1676,8 @@
       <c r="R35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="23"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1698,10 +1698,10 @@
       <c r="R36" s="5"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="20">
+      <c r="A37" s="25">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="16" t="s">
@@ -1724,8 +1724,8 @@
       <c r="R37" s="5"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="23"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="1" t="s">
         <v>18</v>
       </c>
@@ -1746,10 +1746,10 @@
       <c r="R38" s="5"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="20">
+      <c r="A39" s="25">
         <v>4.7</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -1772,8 +1772,8 @@
       <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1794,10 +1794,10 @@
       <c r="R40" s="5"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="20">
+      <c r="A41" s="25">
         <v>4.8</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="16" t="s">
@@ -1820,8 +1820,8 @@
       <c r="R41" s="5"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="23"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="1" t="s">
         <v>18</v>
       </c>
@@ -1860,16 +1860,16 @@
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
       <c r="Q43" s="13"/>
       <c r="R43" s="14"/>
     </row>
     <row r="44" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="20">
+      <c r="A44" s="25">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="16" t="s">
@@ -1892,8 +1892,8 @@
       <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="1" t="s">
         <v>18</v>
       </c>
@@ -1933,15 +1933,15 @@
       <c r="M46" s="13"/>
       <c r="N46" s="13"/>
       <c r="O46" s="13"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="38"/>
-      <c r="R46" s="39"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="20">
+      <c r="A47" s="25">
         <v>6.1</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -1964,8 +1964,8 @@
       <c r="R47" s="5"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
-      <c r="B48" s="23"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="1" t="s">
         <v>18</v>
       </c>
@@ -1986,10 +1986,10 @@
       <c r="R48" s="5"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="20">
+      <c r="A49" s="25">
         <v>6.2</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="27" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="16" t="s">
@@ -2012,8 +2012,8 @@
       <c r="R49" s="5"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="23"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="1" t="s">
         <v>18</v>
       </c>
@@ -2034,10 +2034,10 @@
       <c r="R50" s="5"/>
     </row>
     <row r="51" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20">
+      <c r="A51" s="25">
         <v>6.3</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="27" t="s">
         <v>34</v>
       </c>
       <c r="C51" s="16" t="s">
@@ -2060,8 +2060,8 @@
       <c r="R51" s="12"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="23"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="1" t="s">
         <v>18</v>
       </c>
@@ -2082,10 +2082,10 @@
       <c r="R52" s="5"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="20">
+      <c r="A53" s="25">
         <v>6.4</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C53" s="16" t="s">
@@ -2108,8 +2108,8 @@
       <c r="R53" s="12"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="23"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="1" t="s">
         <v>18</v>
       </c>
@@ -2154,10 +2154,10 @@
       <c r="R55" s="14"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="20">
+      <c r="A56" s="25">
         <v>7.1</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C56" t="s">
@@ -2180,8 +2180,8 @@
       <c r="R56" s="12"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="1" t="s">
         <v>18</v>
       </c>
@@ -2202,10 +2202,10 @@
       <c r="R57" s="5"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A58" s="20">
+      <c r="A58" s="25">
         <v>7.2</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="27" t="s">
         <v>36</v>
       </c>
       <c r="C58" t="s">
@@ -2228,8 +2228,8 @@
       <c r="R58" s="5"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="21"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
@@ -2251,6 +2251,57 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
@@ -2267,57 +2318,6 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>

</xml_diff>